<commit_message>
ACM To BTK Converter linkleri donusturucu dosyasına eklendi.
</commit_message>
<xml_diff>
--- a/pages/donusturucu.xlsx
+++ b/pages/donusturucu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Sıra</t>
   </si>
@@ -99,13 +99,16 @@
   </si>
   <si>
     <t>Model-01</t>
+  </si>
+  <si>
+    <t>https://github.com/btk42/CV-ATB-00-000-MCR-S2B0-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -137,6 +140,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="162"/>
     </font>
@@ -173,10 +184,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -196,8 +208,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,7 +495,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -597,7 +613,9 @@
       <c r="J3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -633,8 +651,11 @@
       <c r="K4" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>

</xml_diff>